<commit_message>
modify optimum score analysis
</commit_message>
<xml_diff>
--- a/2/score.xlsx
+++ b/2/score.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="5610" firstSheet="11" activeTab="11"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="5610"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -2839,7 +2839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
@@ -5513,7 +5513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>

</xml_diff>